<commit_message>
fixing metrics df name
Signed-off-by: Felipe Campos <fepas.unb@gmail.com>
</commit_message>
<xml_diff>
--- a/data/metrics_df.xlsx
+++ b/data/metrics_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,20 +464,30 @@
           <t>asc1</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ac1</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>total</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.6</v>
+        <v>0.9666666666666667</v>
       </c>
       <c r="B2" t="n">
-        <v>0.2</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>etl_news</t>
+          <t>frontend</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -486,22 +496,28 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.5940000000000001</v>
+        <v>0.671</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.671</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.671</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.6</v>
+        <v>0.9666666666666667</v>
       </c>
       <c r="B3" t="n">
-        <v>0.2</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>etl_news</t>
+          <t>frontend</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -510,22 +526,28 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.5940000000000001</v>
+        <v>0.671</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.671</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.671</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.6</v>
+        <v>0.9666666666666667</v>
       </c>
       <c r="B4" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>etl_news</t>
+          <t>frontend</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -534,22 +556,28 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.5940000000000001</v>
+        <v>0.6819999999999999</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.6819999999999999</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.6819999999999999</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.6</v>
+        <v>0.96875</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2</v>
+        <v>0.09375</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0.9375</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>etl_news</t>
+          <t>frontend</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -558,22 +586,28 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.5940000000000001</v>
+        <v>0.66</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.66</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.6</v>
+        <v>0.96875</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2</v>
+        <v>0.09375</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>0.9375</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>etl_news</t>
+          <t>frontend</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -582,22 +616,28 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0.5940000000000001</v>
+        <v>0.66</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.66</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.6</v>
+        <v>0.96875</v>
       </c>
       <c r="B7" t="n">
-        <v>0.2</v>
+        <v>0.09375</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0.9375</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>etl_news</t>
+          <t>frontend</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -606,22 +646,28 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0.5940000000000001</v>
+        <v>0.66</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.66</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.6</v>
+        <v>0.96875</v>
       </c>
       <c r="B8" t="n">
-        <v>0.2</v>
+        <v>0.0625</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>0.9375</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>etl_news</t>
+          <t>frontend</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -630,22 +676,28 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0.5940000000000001</v>
+        <v>0.6496875</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.6496875</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.6496875</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.6</v>
+        <v>0.9714285714285714</v>
       </c>
       <c r="B9" t="n">
-        <v>0.2</v>
+        <v>0.05714285714285714</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0.9714285714285714</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>etl_news</t>
+          <t>frontend</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -654,22 +706,28 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>0.5940000000000001</v>
+        <v>0.6599999999999999</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.6599999999999999</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.6599999999999999</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.6</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="B10" t="n">
-        <v>0.2</v>
+        <v>0.1071428571428571</v>
       </c>
       <c r="C10" t="n">
         <v>1</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>etl_news</t>
+          <t>frontend</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -678,30 +736,1542 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0.5940000000000001</v>
+        <v>0.6835714285714286</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.6835714285714286</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.6835714285714286</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.6</v>
+        <v>0.9375</v>
       </c>
       <c r="B11" t="n">
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
       <c r="C11" t="n">
         <v>1</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
+          <t>frontend</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>23-03-2021</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>0.680625</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.680625</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.680625</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>gateway</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>01-05-2021</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>gateway</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>02-05-2021</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>gateway</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>04-05-2021</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>gateway</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>09-05-2021</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>gateway</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>09-05-2021(1)</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>gateway</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>09-05-2021(2)</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>gateway</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>10-05-2021</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>gateway</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>10-05-2021(1)</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>gateway</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>18-04-2021</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>gateway</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>23-03-2021</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>etl_tse</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>01-05-2021</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.528</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>etl_tse</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>02-05-2021</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.528</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>etl_tse</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>04-05-2021</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.528</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>etl_tse</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>09-05-2021</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.528</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>etl_tse</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>09-05-2021(1)</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.528</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>etl_tse</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>09-05-2021(2)</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.528</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>etl_tse</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>10-05-2021</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.528</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>etl_tse</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>10-05-2021(1)</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.528</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>etl_tse</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>18-04-2021</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.528</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>etl_tse</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>23-03-2021</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.528</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>etl_twitter</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>01-05-2021</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>etl_twitter</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>02-05-2021</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>etl_twitter</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>04-05-2021</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>etl_twitter</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>09-05-2021</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>etl_twitter</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>09-05-2021(1)</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B37" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>etl_twitter</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>09-05-2021(2)</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>etl_twitter</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>10-05-2021</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>etl_twitter</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>10-05-2021(1)</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>etl_twitter</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>18-04-2021</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>etl_twitter</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>23-03-2021</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0.528</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>etl_camara</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>01-05-2021</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C43" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>etl_camara</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>02-05-2021</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C44" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>etl_camara</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>04-05-2021</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B45" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>etl_camara</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>09-05-2021</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B46" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>etl_camara</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>09-05-2021(1)</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B47" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C47" t="n">
+        <v>1</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>etl_camara</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>09-05-2021(2)</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B48" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C48" t="n">
+        <v>1</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>etl_camara</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>10-05-2021</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B49" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C49" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>etl_camara</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>10-05-2021(1)</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B50" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>etl_camara</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>18-04-2021</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B51" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C51" t="n">
+        <v>1</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>etl_camara</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>23-03-2021</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B52" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
           <t>etl_news</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>01-05-2021</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B53" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C53" t="n">
+        <v>1</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>etl_news</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>02-05-2021</t>
+        </is>
+      </c>
+      <c r="F53" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B54" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C54" t="n">
+        <v>1</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>etl_news</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>04-05-2021</t>
+        </is>
+      </c>
+      <c r="F54" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B55" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C55" t="n">
+        <v>1</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>etl_news</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>09-05-2021</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B56" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>etl_news</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>09-05-2021(1)</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B57" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C57" t="n">
+        <v>1</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>etl_news</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>09-05-2021(2)</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B58" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C58" t="n">
+        <v>1</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>etl_news</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>10-05-2021</t>
+        </is>
+      </c>
+      <c r="F58" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B59" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C59" t="n">
+        <v>1</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>etl_news</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>10-05-2021(1)</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B60" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C60" t="n">
+        <v>1</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>etl_news</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>18-04-2021</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B61" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>etl_news</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
         <is>
           <t>23-03-2021</t>
         </is>
       </c>
-      <c r="F11" t="n">
+      <c r="F61" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H61" t="n">
         <v>0.5940000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding analisys all repos
Signed-off-by: Felipe Campos <fepas.unb@gmail.com>
</commit_message>
<xml_diff>
--- a/data/metrics_df.xlsx
+++ b/data/metrics_df.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,15 +465,20 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>ncloc</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>asc1</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>ac1</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>total</t>
         </is>
@@ -498,12 +503,15 @@
         <v>44278</v>
       </c>
       <c r="F2" t="n">
-        <v>0.680625</v>
+        <v>522</v>
       </c>
       <c r="G2" t="n">
         <v>0.680625</v>
       </c>
       <c r="H2" t="n">
+        <v>0.680625</v>
+      </c>
+      <c r="I2" t="n">
         <v>0.680625</v>
       </c>
     </row>
@@ -526,12 +534,15 @@
         <v>44304</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6835714285714286</v>
+        <v>1242</v>
       </c>
       <c r="G3" t="n">
         <v>0.6835714285714286</v>
       </c>
       <c r="H3" t="n">
+        <v>0.6835714285714286</v>
+      </c>
+      <c r="I3" t="n">
         <v>0.6835714285714286</v>
       </c>
     </row>
@@ -554,12 +565,15 @@
         <v>44317</v>
       </c>
       <c r="F4" t="n">
-        <v>0.671</v>
+        <v>1406</v>
       </c>
       <c r="G4" t="n">
         <v>0.671</v>
       </c>
       <c r="H4" t="n">
+        <v>0.671</v>
+      </c>
+      <c r="I4" t="n">
         <v>0.671</v>
       </c>
     </row>
@@ -582,12 +596,15 @@
         <v>44318</v>
       </c>
       <c r="F5" t="n">
-        <v>0.671</v>
+        <v>1406</v>
       </c>
       <c r="G5" t="n">
         <v>0.671</v>
       </c>
       <c r="H5" t="n">
+        <v>0.671</v>
+      </c>
+      <c r="I5" t="n">
         <v>0.671</v>
       </c>
     </row>
@@ -610,12 +627,15 @@
         <v>44320</v>
       </c>
       <c r="F6" t="n">
-        <v>0.6819999999999999</v>
+        <v>1392</v>
       </c>
       <c r="G6" t="n">
         <v>0.6819999999999999</v>
       </c>
       <c r="H6" t="n">
+        <v>0.6819999999999999</v>
+      </c>
+      <c r="I6" t="n">
         <v>0.6819999999999999</v>
       </c>
     </row>
@@ -638,12 +658,15 @@
         <v>44325</v>
       </c>
       <c r="F7" t="n">
-        <v>0.66</v>
+        <v>1780</v>
       </c>
       <c r="G7" t="n">
         <v>0.66</v>
       </c>
       <c r="H7" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="I7" t="n">
         <v>0.66</v>
       </c>
     </row>
@@ -666,12 +689,15 @@
         <v>44325.04166666666</v>
       </c>
       <c r="F8" t="n">
-        <v>0.66</v>
+        <v>1780</v>
       </c>
       <c r="G8" t="n">
         <v>0.66</v>
       </c>
       <c r="H8" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="I8" t="n">
         <v>0.66</v>
       </c>
     </row>
@@ -694,12 +720,15 @@
         <v>44325.08333333334</v>
       </c>
       <c r="F9" t="n">
-        <v>0.66</v>
+        <v>1780</v>
       </c>
       <c r="G9" t="n">
         <v>0.66</v>
       </c>
       <c r="H9" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="I9" t="n">
         <v>0.66</v>
       </c>
     </row>
@@ -722,12 +751,15 @@
         <v>44326</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6496875</v>
+        <v>1842</v>
       </c>
       <c r="G10" t="n">
         <v>0.6496875</v>
       </c>
       <c r="H10" t="n">
+        <v>0.6496875</v>
+      </c>
+      <c r="I10" t="n">
         <v>0.6496875</v>
       </c>
     </row>
@@ -750,7 +782,7 @@
         <v>44326.04166666666</v>
       </c>
       <c r="F11" t="n">
-        <v>0.6599999999999999</v>
+        <v>2052</v>
       </c>
       <c r="G11" t="n">
         <v>0.6599999999999999</v>
@@ -758,33 +790,39 @@
       <c r="H11" t="n">
         <v>0.6599999999999999</v>
       </c>
+      <c r="I11" t="n">
+        <v>0.6599999999999999</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.972972972972973</v>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>0.05405405405405406</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>0.972972972972973</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>gateway</t>
+          <t>frontend</t>
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>44278</v>
+        <v>44335</v>
       </c>
       <c r="F12" t="n">
-        <v>0.5133333333333334</v>
+        <v>2289</v>
       </c>
       <c r="G12" t="n">
-        <v>0.5133333333333334</v>
+        <v>0.6600000000000001</v>
       </c>
       <c r="H12" t="n">
-        <v>0.5133333333333334</v>
+        <v>0.6600000000000001</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.6600000000000001</v>
       </c>
     </row>
     <row r="13">
@@ -803,15 +841,18 @@
         </is>
       </c>
       <c r="E13" s="2" t="n">
-        <v>44304</v>
+        <v>44278</v>
       </c>
       <c r="F13" t="n">
-        <v>0.5133333333333334</v>
+        <v>89</v>
       </c>
       <c r="G13" t="n">
         <v>0.5133333333333334</v>
       </c>
       <c r="H13" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="I13" t="n">
         <v>0.5133333333333334</v>
       </c>
     </row>
@@ -831,15 +872,18 @@
         </is>
       </c>
       <c r="E14" s="2" t="n">
-        <v>44317</v>
+        <v>44304</v>
       </c>
       <c r="F14" t="n">
-        <v>0.5133333333333334</v>
+        <v>116</v>
       </c>
       <c r="G14" t="n">
         <v>0.5133333333333334</v>
       </c>
       <c r="H14" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="I14" t="n">
         <v>0.5133333333333334</v>
       </c>
     </row>
@@ -859,15 +903,18 @@
         </is>
       </c>
       <c r="E15" s="2" t="n">
-        <v>44318</v>
+        <v>44317</v>
       </c>
       <c r="F15" t="n">
-        <v>0.5133333333333334</v>
+        <v>128</v>
       </c>
       <c r="G15" t="n">
         <v>0.5133333333333334</v>
       </c>
       <c r="H15" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="I15" t="n">
         <v>0.5133333333333334</v>
       </c>
     </row>
@@ -887,15 +934,18 @@
         </is>
       </c>
       <c r="E16" s="2" t="n">
-        <v>44320</v>
+        <v>44318</v>
       </c>
       <c r="F16" t="n">
-        <v>0.5133333333333334</v>
+        <v>128</v>
       </c>
       <c r="G16" t="n">
         <v>0.5133333333333334</v>
       </c>
       <c r="H16" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="I16" t="n">
         <v>0.5133333333333334</v>
       </c>
     </row>
@@ -915,15 +965,18 @@
         </is>
       </c>
       <c r="E17" s="2" t="n">
-        <v>44325</v>
+        <v>44320</v>
       </c>
       <c r="F17" t="n">
-        <v>0.5133333333333334</v>
+        <v>128</v>
       </c>
       <c r="G17" t="n">
         <v>0.5133333333333334</v>
       </c>
       <c r="H17" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="I17" t="n">
         <v>0.5133333333333334</v>
       </c>
     </row>
@@ -943,15 +996,18 @@
         </is>
       </c>
       <c r="E18" s="2" t="n">
-        <v>44325.04166666666</v>
+        <v>44325</v>
       </c>
       <c r="F18" t="n">
-        <v>0.5133333333333334</v>
+        <v>128</v>
       </c>
       <c r="G18" t="n">
         <v>0.5133333333333334</v>
       </c>
       <c r="H18" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="I18" t="n">
         <v>0.5133333333333334</v>
       </c>
     </row>
@@ -971,15 +1027,18 @@
         </is>
       </c>
       <c r="E19" s="2" t="n">
-        <v>44325.08333333334</v>
+        <v>44325.04166666666</v>
       </c>
       <c r="F19" t="n">
-        <v>0.5133333333333334</v>
+        <v>132</v>
       </c>
       <c r="G19" t="n">
         <v>0.5133333333333334</v>
       </c>
       <c r="H19" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="I19" t="n">
         <v>0.5133333333333334</v>
       </c>
     </row>
@@ -999,15 +1058,18 @@
         </is>
       </c>
       <c r="E20" s="2" t="n">
-        <v>44326</v>
+        <v>44325.08333333334</v>
       </c>
       <c r="F20" t="n">
-        <v>0.5133333333333334</v>
+        <v>132</v>
       </c>
       <c r="G20" t="n">
         <v>0.5133333333333334</v>
       </c>
       <c r="H20" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="I20" t="n">
         <v>0.5133333333333334</v>
       </c>
     </row>
@@ -1027,21 +1089,24 @@
         </is>
       </c>
       <c r="E21" s="2" t="n">
-        <v>44326.04166666666</v>
+        <v>44326</v>
       </c>
       <c r="F21" t="n">
-        <v>0.5133333333333334</v>
+        <v>136</v>
       </c>
       <c r="G21" t="n">
         <v>0.5133333333333334</v>
       </c>
       <c r="H21" t="n">
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="I21" t="n">
         <v>0.5133333333333334</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.6</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="B22" t="n">
         <v>0</v>
@@ -1051,20 +1116,23 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>etl_tse</t>
+          <t>gateway</t>
         </is>
       </c>
       <c r="E22" s="2" t="n">
-        <v>44278</v>
+        <v>44326.04166666666</v>
       </c>
       <c r="F22" t="n">
-        <v>0.528</v>
+        <v>136</v>
       </c>
       <c r="G22" t="n">
-        <v>0.528</v>
+        <v>0.5133333333333334</v>
       </c>
       <c r="H22" t="n">
-        <v>0.528</v>
+        <v>0.5133333333333334</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.5133333333333334</v>
       </c>
     </row>
     <row r="23">
@@ -1079,19 +1147,22 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>etl_tse</t>
+          <t>gateway</t>
         </is>
       </c>
       <c r="E23" s="2" t="n">
-        <v>44304</v>
+        <v>44335</v>
       </c>
       <c r="F23" t="n">
-        <v>0.528</v>
+        <v>280</v>
       </c>
       <c r="G23" t="n">
         <v>0.528</v>
       </c>
       <c r="H23" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="I23" t="n">
         <v>0.528</v>
       </c>
     </row>
@@ -1111,15 +1182,18 @@
         </is>
       </c>
       <c r="E24" s="2" t="n">
-        <v>44317</v>
+        <v>44278</v>
       </c>
       <c r="F24" t="n">
-        <v>0.528</v>
+        <v>97</v>
       </c>
       <c r="G24" t="n">
         <v>0.528</v>
       </c>
       <c r="H24" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="I24" t="n">
         <v>0.528</v>
       </c>
     </row>
@@ -1139,15 +1213,18 @@
         </is>
       </c>
       <c r="E25" s="2" t="n">
-        <v>44318</v>
+        <v>44304</v>
       </c>
       <c r="F25" t="n">
-        <v>0.528</v>
+        <v>97</v>
       </c>
       <c r="G25" t="n">
         <v>0.528</v>
       </c>
       <c r="H25" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="I25" t="n">
         <v>0.528</v>
       </c>
     </row>
@@ -1167,15 +1244,18 @@
         </is>
       </c>
       <c r="E26" s="2" t="n">
-        <v>44320</v>
+        <v>44317</v>
       </c>
       <c r="F26" t="n">
-        <v>0.528</v>
+        <v>97</v>
       </c>
       <c r="G26" t="n">
         <v>0.528</v>
       </c>
       <c r="H26" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="I26" t="n">
         <v>0.528</v>
       </c>
     </row>
@@ -1195,15 +1275,18 @@
         </is>
       </c>
       <c r="E27" s="2" t="n">
-        <v>44325</v>
+        <v>44318</v>
       </c>
       <c r="F27" t="n">
-        <v>0.528</v>
+        <v>97</v>
       </c>
       <c r="G27" t="n">
         <v>0.528</v>
       </c>
       <c r="H27" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="I27" t="n">
         <v>0.528</v>
       </c>
     </row>
@@ -1223,15 +1306,18 @@
         </is>
       </c>
       <c r="E28" s="2" t="n">
-        <v>44325.04166666666</v>
+        <v>44320</v>
       </c>
       <c r="F28" t="n">
-        <v>0.528</v>
+        <v>97</v>
       </c>
       <c r="G28" t="n">
         <v>0.528</v>
       </c>
       <c r="H28" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="I28" t="n">
         <v>0.528</v>
       </c>
     </row>
@@ -1251,15 +1337,18 @@
         </is>
       </c>
       <c r="E29" s="2" t="n">
-        <v>44325.08333333334</v>
+        <v>44325</v>
       </c>
       <c r="F29" t="n">
-        <v>0.528</v>
+        <v>98</v>
       </c>
       <c r="G29" t="n">
         <v>0.528</v>
       </c>
       <c r="H29" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="I29" t="n">
         <v>0.528</v>
       </c>
     </row>
@@ -1279,15 +1368,18 @@
         </is>
       </c>
       <c r="E30" s="2" t="n">
-        <v>44326</v>
+        <v>44325.04166666666</v>
       </c>
       <c r="F30" t="n">
-        <v>0.528</v>
+        <v>98</v>
       </c>
       <c r="G30" t="n">
         <v>0.528</v>
       </c>
       <c r="H30" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="I30" t="n">
         <v>0.528</v>
       </c>
     </row>
@@ -1307,43 +1399,49 @@
         </is>
       </c>
       <c r="E31" s="2" t="n">
-        <v>44326.04166666666</v>
+        <v>44325.08333333334</v>
       </c>
       <c r="F31" t="n">
-        <v>0.528</v>
+        <v>98</v>
       </c>
       <c r="G31" t="n">
         <v>0.528</v>
       </c>
       <c r="H31" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="I31" t="n">
         <v>0.528</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="B32" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
         <v>1</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>etl_twitter</t>
+          <t>etl_tse</t>
         </is>
       </c>
       <c r="E32" s="2" t="n">
-        <v>44278</v>
+        <v>44326</v>
       </c>
       <c r="F32" t="n">
-        <v>0.528</v>
+        <v>98</v>
       </c>
       <c r="G32" t="n">
         <v>0.528</v>
       </c>
       <c r="H32" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="I32" t="n">
         <v>0.528</v>
       </c>
     </row>
@@ -1352,63 +1450,69 @@
         <v>0.6</v>
       </c>
       <c r="B33" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="C33" t="n">
         <v>1</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>etl_twitter</t>
+          <t>etl_tse</t>
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>44304</v>
+        <v>44326.04166666666</v>
       </c>
       <c r="F33" t="n">
-        <v>0.66</v>
+        <v>98</v>
       </c>
       <c r="G33" t="n">
-        <v>0.66</v>
+        <v>0.528</v>
       </c>
       <c r="H33" t="n">
-        <v>0.66</v>
+        <v>0.528</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.528</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.6</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="C34" t="n">
         <v>1</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>etl_twitter</t>
+          <t>etl_tse</t>
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>44317</v>
+        <v>44335</v>
       </c>
       <c r="F34" t="n">
-        <v>0.66</v>
+        <v>128</v>
       </c>
       <c r="G34" t="n">
-        <v>0.66</v>
+        <v>0.55</v>
       </c>
       <c r="H34" t="n">
-        <v>0.66</v>
+        <v>0.55</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.55</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="B35" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="C35" t="n">
         <v>1</v>
@@ -1419,16 +1523,19 @@
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>44318</v>
+        <v>44278</v>
       </c>
       <c r="F35" t="n">
-        <v>0.66</v>
+        <v>62</v>
       </c>
       <c r="G35" t="n">
-        <v>0.66</v>
+        <v>0.528</v>
       </c>
       <c r="H35" t="n">
-        <v>0.66</v>
+        <v>0.528</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.528</v>
       </c>
     </row>
     <row r="36">
@@ -1447,10 +1554,10 @@
         </is>
       </c>
       <c r="E36" s="2" t="n">
-        <v>44320</v>
+        <v>44304</v>
       </c>
       <c r="F36" t="n">
-        <v>0.66</v>
+        <v>209</v>
       </c>
       <c r="G36" t="n">
         <v>0.66</v>
@@ -1458,6 +1565,9 @@
       <c r="H36" t="n">
         <v>0.66</v>
       </c>
+      <c r="I36" t="n">
+        <v>0.66</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1475,10 +1585,10 @@
         </is>
       </c>
       <c r="E37" s="2" t="n">
-        <v>44325</v>
+        <v>44317</v>
       </c>
       <c r="F37" t="n">
-        <v>0.66</v>
+        <v>209</v>
       </c>
       <c r="G37" t="n">
         <v>0.66</v>
@@ -1486,13 +1596,16 @@
       <c r="H37" t="n">
         <v>0.66</v>
       </c>
+      <c r="I37" t="n">
+        <v>0.66</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
         <v>0.6</v>
       </c>
       <c r="B38" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="C38" t="n">
         <v>1</v>
@@ -1503,16 +1616,19 @@
         </is>
       </c>
       <c r="E38" s="2" t="n">
-        <v>44325.04166666666</v>
+        <v>44318</v>
       </c>
       <c r="F38" t="n">
-        <v>0.5940000000000001</v>
+        <v>209</v>
       </c>
       <c r="G38" t="n">
-        <v>0.5940000000000001</v>
+        <v>0.66</v>
       </c>
       <c r="H38" t="n">
-        <v>0.5940000000000001</v>
+        <v>0.66</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0.66</v>
       </c>
     </row>
     <row r="39">
@@ -1520,7 +1636,7 @@
         <v>0.6</v>
       </c>
       <c r="B39" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="C39" t="n">
         <v>1</v>
@@ -1531,16 +1647,19 @@
         </is>
       </c>
       <c r="E39" s="2" t="n">
-        <v>44325.08333333334</v>
+        <v>44320</v>
       </c>
       <c r="F39" t="n">
-        <v>0.5940000000000001</v>
+        <v>209</v>
       </c>
       <c r="G39" t="n">
-        <v>0.5940000000000001</v>
+        <v>0.66</v>
       </c>
       <c r="H39" t="n">
-        <v>0.5940000000000001</v>
+        <v>0.66</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0.66</v>
       </c>
     </row>
     <row r="40">
@@ -1548,7 +1667,7 @@
         <v>0.6</v>
       </c>
       <c r="B40" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="C40" t="n">
         <v>1</v>
@@ -1559,16 +1678,19 @@
         </is>
       </c>
       <c r="E40" s="2" t="n">
-        <v>44326</v>
+        <v>44325</v>
       </c>
       <c r="F40" t="n">
-        <v>0.5940000000000001</v>
+        <v>209</v>
       </c>
       <c r="G40" t="n">
-        <v>0.5940000000000001</v>
+        <v>0.66</v>
       </c>
       <c r="H40" t="n">
-        <v>0.5940000000000001</v>
+        <v>0.66</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0.66</v>
       </c>
     </row>
     <row r="41">
@@ -1587,15 +1709,18 @@
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>44326.04166666666</v>
+        <v>44325.04166666666</v>
       </c>
       <c r="F41" t="n">
-        <v>0.5940000000000001</v>
+        <v>322</v>
       </c>
       <c r="G41" t="n">
         <v>0.5940000000000001</v>
       </c>
       <c r="H41" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="I41" t="n">
         <v>0.5940000000000001</v>
       </c>
     </row>
@@ -1611,19 +1736,22 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>etl_camara</t>
+          <t>etl_twitter</t>
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>44278</v>
+        <v>44325.08333333334</v>
       </c>
       <c r="F42" t="n">
-        <v>0.5940000000000001</v>
+        <v>322</v>
       </c>
       <c r="G42" t="n">
         <v>0.5940000000000001</v>
       </c>
       <c r="H42" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="I42" t="n">
         <v>0.5940000000000001</v>
       </c>
     </row>
@@ -1639,19 +1767,22 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>etl_camara</t>
+          <t>etl_twitter</t>
         </is>
       </c>
       <c r="E43" s="2" t="n">
-        <v>44304</v>
+        <v>44326</v>
       </c>
       <c r="F43" t="n">
-        <v>0.5940000000000001</v>
+        <v>329</v>
       </c>
       <c r="G43" t="n">
         <v>0.5940000000000001</v>
       </c>
       <c r="H43" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="I43" t="n">
         <v>0.5940000000000001</v>
       </c>
     </row>
@@ -1667,48 +1798,54 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>etl_camara</t>
+          <t>etl_twitter</t>
         </is>
       </c>
       <c r="E44" s="2" t="n">
-        <v>44317</v>
+        <v>44326.04166666666</v>
       </c>
       <c r="F44" t="n">
-        <v>0.5940000000000001</v>
+        <v>329</v>
       </c>
       <c r="G44" t="n">
         <v>0.5940000000000001</v>
       </c>
       <c r="H44" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="I44" t="n">
         <v>0.5940000000000001</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>0.6</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="B45" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C45" t="n">
         <v>1</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>etl_camara</t>
+          <t>etl_twitter</t>
         </is>
       </c>
       <c r="E45" s="2" t="n">
-        <v>44318</v>
+        <v>44335</v>
       </c>
       <c r="F45" t="n">
-        <v>0.5940000000000001</v>
+        <v>398</v>
       </c>
       <c r="G45" t="n">
-        <v>0.5940000000000001</v>
+        <v>0.55</v>
       </c>
       <c r="H45" t="n">
-        <v>0.5940000000000001</v>
+        <v>0.55</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0.55</v>
       </c>
     </row>
     <row r="46">
@@ -1727,15 +1864,18 @@
         </is>
       </c>
       <c r="E46" s="2" t="n">
-        <v>44320</v>
+        <v>44278</v>
       </c>
       <c r="F46" t="n">
-        <v>0.5940000000000001</v>
+        <v>122</v>
       </c>
       <c r="G46" t="n">
         <v>0.5940000000000001</v>
       </c>
       <c r="H46" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="I46" t="n">
         <v>0.5940000000000001</v>
       </c>
     </row>
@@ -1755,15 +1895,18 @@
         </is>
       </c>
       <c r="E47" s="2" t="n">
-        <v>44325</v>
+        <v>44304</v>
       </c>
       <c r="F47" t="n">
-        <v>0.5940000000000001</v>
+        <v>403</v>
       </c>
       <c r="G47" t="n">
         <v>0.5940000000000001</v>
       </c>
       <c r="H47" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="I47" t="n">
         <v>0.5940000000000001</v>
       </c>
     </row>
@@ -1783,15 +1926,18 @@
         </is>
       </c>
       <c r="E48" s="2" t="n">
-        <v>44325.04166666666</v>
+        <v>44317</v>
       </c>
       <c r="F48" t="n">
-        <v>0.5940000000000001</v>
+        <v>525</v>
       </c>
       <c r="G48" t="n">
         <v>0.5940000000000001</v>
       </c>
       <c r="H48" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="I48" t="n">
         <v>0.5940000000000001</v>
       </c>
     </row>
@@ -1811,15 +1957,18 @@
         </is>
       </c>
       <c r="E49" s="2" t="n">
-        <v>44325.08333333334</v>
+        <v>44318</v>
       </c>
       <c r="F49" t="n">
-        <v>0.5940000000000001</v>
+        <v>525</v>
       </c>
       <c r="G49" t="n">
         <v>0.5940000000000001</v>
       </c>
       <c r="H49" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="I49" t="n">
         <v>0.5940000000000001</v>
       </c>
     </row>
@@ -1839,15 +1988,18 @@
         </is>
       </c>
       <c r="E50" s="2" t="n">
-        <v>44326</v>
+        <v>44320</v>
       </c>
       <c r="F50" t="n">
-        <v>0.5940000000000001</v>
+        <v>525</v>
       </c>
       <c r="G50" t="n">
         <v>0.5940000000000001</v>
       </c>
       <c r="H50" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="I50" t="n">
         <v>0.5940000000000001</v>
       </c>
     </row>
@@ -1867,15 +2019,18 @@
         </is>
       </c>
       <c r="E51" s="2" t="n">
-        <v>44326.04166666666</v>
+        <v>44325</v>
       </c>
       <c r="F51" t="n">
-        <v>0.5940000000000001</v>
+        <v>525</v>
       </c>
       <c r="G51" t="n">
         <v>0.5940000000000001</v>
       </c>
       <c r="H51" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="I51" t="n">
         <v>0.5940000000000001</v>
       </c>
     </row>
@@ -1891,19 +2046,22 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>etl_news</t>
+          <t>etl_camara</t>
         </is>
       </c>
       <c r="E52" s="2" t="n">
-        <v>44304</v>
+        <v>44325.04166666666</v>
       </c>
       <c r="F52" t="n">
-        <v>0.5940000000000001</v>
+        <v>525</v>
       </c>
       <c r="G52" t="n">
         <v>0.5940000000000001</v>
       </c>
       <c r="H52" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="I52" t="n">
         <v>0.5940000000000001</v>
       </c>
     </row>
@@ -1919,19 +2077,22 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>etl_news</t>
+          <t>etl_camara</t>
         </is>
       </c>
       <c r="E53" s="2" t="n">
-        <v>44317</v>
+        <v>44325.08333333334</v>
       </c>
       <c r="F53" t="n">
-        <v>0.5940000000000001</v>
+        <v>525</v>
       </c>
       <c r="G53" t="n">
         <v>0.5940000000000001</v>
       </c>
       <c r="H53" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="I53" t="n">
         <v>0.5940000000000001</v>
       </c>
     </row>
@@ -1947,19 +2108,22 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>etl_news</t>
+          <t>etl_camara</t>
         </is>
       </c>
       <c r="E54" s="2" t="n">
-        <v>44318</v>
+        <v>44326</v>
       </c>
       <c r="F54" t="n">
-        <v>0.5940000000000001</v>
+        <v>525</v>
       </c>
       <c r="G54" t="n">
         <v>0.5940000000000001</v>
       </c>
       <c r="H54" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="I54" t="n">
         <v>0.5940000000000001</v>
       </c>
     </row>
@@ -1975,48 +2139,54 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>etl_news</t>
+          <t>etl_camara</t>
         </is>
       </c>
       <c r="E55" s="2" t="n">
-        <v>44320</v>
+        <v>44326.04166666666</v>
       </c>
       <c r="F55" t="n">
-        <v>0.5940000000000001</v>
+        <v>525</v>
       </c>
       <c r="G55" t="n">
         <v>0.5940000000000001</v>
       </c>
       <c r="H55" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="I55" t="n">
         <v>0.5940000000000001</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>0.6</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="B56" t="n">
-        <v>0.2</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="C56" t="n">
         <v>1</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>etl_news</t>
+          <t>etl_camara</t>
         </is>
       </c>
       <c r="E56" s="2" t="n">
-        <v>44325</v>
+        <v>44335</v>
       </c>
       <c r="F56" t="n">
-        <v>0.5940000000000001</v>
+        <v>844</v>
       </c>
       <c r="G56" t="n">
-        <v>0.5940000000000001</v>
+        <v>0.605</v>
       </c>
       <c r="H56" t="n">
-        <v>0.5940000000000001</v>
+        <v>0.605</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0.605</v>
       </c>
     </row>
     <row r="57">
@@ -2035,15 +2205,18 @@
         </is>
       </c>
       <c r="E57" s="2" t="n">
-        <v>44325.04166666666</v>
+        <v>44304</v>
       </c>
       <c r="F57" t="n">
-        <v>0.5940000000000001</v>
+        <v>164</v>
       </c>
       <c r="G57" t="n">
         <v>0.5940000000000001</v>
       </c>
       <c r="H57" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="I57" t="n">
         <v>0.5940000000000001</v>
       </c>
     </row>
@@ -2063,15 +2236,18 @@
         </is>
       </c>
       <c r="E58" s="2" t="n">
-        <v>44325.08333333334</v>
+        <v>44317</v>
       </c>
       <c r="F58" t="n">
-        <v>0.5940000000000001</v>
+        <v>164</v>
       </c>
       <c r="G58" t="n">
         <v>0.5940000000000001</v>
       </c>
       <c r="H58" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="I58" t="n">
         <v>0.5940000000000001</v>
       </c>
     </row>
@@ -2091,15 +2267,18 @@
         </is>
       </c>
       <c r="E59" s="2" t="n">
-        <v>44326</v>
+        <v>44318</v>
       </c>
       <c r="F59" t="n">
-        <v>0.5940000000000001</v>
+        <v>164</v>
       </c>
       <c r="G59" t="n">
         <v>0.5940000000000001</v>
       </c>
       <c r="H59" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="I59" t="n">
         <v>0.5940000000000001</v>
       </c>
     </row>
@@ -2119,16 +2298,205 @@
         </is>
       </c>
       <c r="E60" s="2" t="n">
+        <v>44320</v>
+      </c>
+      <c r="F60" t="n">
+        <v>164</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B61" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>etl_news</t>
+        </is>
+      </c>
+      <c r="E61" s="2" t="n">
+        <v>44325</v>
+      </c>
+      <c r="F61" t="n">
+        <v>164</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B62" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C62" t="n">
+        <v>1</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>etl_news</t>
+        </is>
+      </c>
+      <c r="E62" s="2" t="n">
+        <v>44325.04166666666</v>
+      </c>
+      <c r="F62" t="n">
+        <v>164</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B63" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C63" t="n">
+        <v>1</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>etl_news</t>
+        </is>
+      </c>
+      <c r="E63" s="2" t="n">
+        <v>44325.08333333334</v>
+      </c>
+      <c r="F63" t="n">
+        <v>164</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B64" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C64" t="n">
+        <v>1</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>etl_news</t>
+        </is>
+      </c>
+      <c r="E64" s="2" t="n">
+        <v>44326</v>
+      </c>
+      <c r="F64" t="n">
+        <v>164</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B65" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C65" t="n">
+        <v>1</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>etl_news</t>
+        </is>
+      </c>
+      <c r="E65" s="2" t="n">
         <v>44326.04166666666</v>
       </c>
-      <c r="F60" t="n">
-        <v>0.5940000000000001</v>
-      </c>
-      <c r="G60" t="n">
-        <v>0.5940000000000001</v>
-      </c>
-      <c r="H60" t="n">
-        <v>0.5940000000000001</v>
+      <c r="F65" t="n">
+        <v>164</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="B66" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+      <c r="C66" t="n">
+        <v>1</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>etl_news</t>
+        </is>
+      </c>
+      <c r="E66" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="F66" t="n">
+        <v>252</v>
+      </c>
+      <c r="G66" t="n">
+        <v>0.605</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0.605</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0.605</v>
       </c>
     </row>
   </sheetData>

</xml_diff>